<commit_message>
formatting the code and added comments
</commit_message>
<xml_diff>
--- a/Database/Dictionary-Coffee-and-Books.xlsx
+++ b/Database/Dictionary-Coffee-and-Books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Web Projects\Coffee and Books bookshop\Coffeee-and-Books-bookshop\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07C1EC4-1234-4858-BC04-1553AF3CDCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14236744-D44D-4A04-9E7B-5165449B7F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F186737C-EDA2-46CA-9043-4A9927A471E4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="104">
   <si>
     <t>attributes</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>TABLE: order_details</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -489,6 +492,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -807,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A324CAB2-490B-426D-AB2D-B48BBA878142}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,66 +1288,90 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+      <c r="A31" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="1"/>
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>5</v>
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="3">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>7</v>
@@ -1345,19 +1379,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C36" s="3">
         <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>7</v>
@@ -1365,274 +1399,312 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C37" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="3">
-        <v>10</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="3">
-        <v>50</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A39" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="3">
-        <v>10</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>7</v>
+      <c r="A40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C41" s="3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>99</v>
+        <v>35</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3">
+        <v>10</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F47" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="3">
-        <v>10</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="3">
-        <v>100</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="3">
-        <v>50</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="3">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="3">
+        <v>100</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="3">
+        <v>50</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C51" s="3">
         <v>50</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
+      <c r="E51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F54" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C55" s="3">
         <v>10</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="D55" s="1"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C56" s="3">
         <v>50</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1717,15 +1789,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D64F00304719264D85478B6C57A341CD" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db4e11acb875dde193c8132970e90170">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="823a6a77-3fa8-4256-ba97-a8b1fde95d14" xmlns:ns3="f4faadfc-5802-4a08-84d6-cea611b28b40" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbcc48fa44768aa1e7914d6def4510e0" ns2:_="" ns3:_="">
     <xsd:import namespace="823a6a77-3fa8-4256-ba97-a8b1fde95d14"/>
@@ -1926,15 +1989,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B000C55E-34BF-4C72-8C11-0878203B1653}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9041E8D6-3A19-4E0F-9D98-0D54E2EA8570}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1951,4 +2015,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B000C55E-34BF-4C72-8C11-0878203B1653}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>